<commit_message>
updated calcs from spx
</commit_message>
<xml_diff>
--- a/excl/Calcs for spx.xlsx
+++ b/excl/Calcs for spx.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25629"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tdruvaskalns\OneDrive - Quadient\Desktop\Priv\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://modulr-my.sharepoint.com/personal/toms_druvaskalns_modulrfinance_com/Documents/Desktop/Practise_Projects/JavaApiForShareApp/excl/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{175B5877-4971-4A94-94D0-DF636698AF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="22" documentId="13_ncr:1_{175B5877-4971-4A94-94D0-DF636698AF8A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{FD5BAD2F-BBDA-4061-B0EC-1838ADA9EB06}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPX calcs" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="74">
   <si>
     <t>Blitz</t>
   </si>
@@ -257,17 +257,21 @@
   </si>
   <si>
     <t>EC2</t>
+  </si>
+  <si>
+    <t>Avg $/SXDT</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="4">
+  <numFmts count="5">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
+    <numFmt numFmtId="170" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -306,18 +310,12 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -400,10 +398,9 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="3" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -421,24 +418,26 @@
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="3" xfId="2" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="10" fontId="0" fillId="5" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="4" borderId="3" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="0" fillId="5" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="170" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -748,7 +747,7 @@
   <dimension ref="B1:U22"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="K23" sqref="K23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -769,7 +768,7 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="9"/>
+      <c r="B1" s="8"/>
       <c r="Q1" t="s">
         <v>0</v>
       </c>
@@ -778,14 +777,14 @@
       </c>
       <c r="T1" s="1">
         <f>SUM(Q2:Q24)</f>
-        <v>457000</v>
-      </c>
-      <c r="U1" s="10" t="s">
+        <v>479000</v>
+      </c>
+      <c r="U1" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="2" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="C2" s="12"/>
+      <c r="C2" s="11"/>
       <c r="N2" t="s">
         <v>20</v>
       </c>
@@ -799,27 +798,30 @@
         <f>SUM(C6:C38)</f>
         <v>370827</v>
       </c>
-      <c r="U2" s="10" t="s">
+      <c r="U2" s="9" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="N3" s="13">
+      <c r="N3" s="12">
         <f>D20*1.05^(120-COUNT(D6:D20))</f>
         <v>622155.56250458804</v>
       </c>
-      <c r="Q3" s="2">
-        <v>150000</v>
+      <c r="Q3" s="25">
+        <v>130000</v>
       </c>
       <c r="S3" t="s">
         <v>19</v>
       </c>
       <c r="T3" s="1">
         <f>T1+T2</f>
-        <v>827827</v>
+        <v>849827</v>
       </c>
     </row>
     <row r="4" spans="2:21" x14ac:dyDescent="0.25">
+      <c r="Q4" s="25">
+        <v>42000</v>
+      </c>
       <c r="S4" t="s">
         <v>17</v>
       </c>
@@ -827,310 +829,317 @@
         <f>SUM(D6:D35)</f>
         <v>46539</v>
       </c>
-      <c r="U4" s="9" t="s">
+      <c r="U4" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" spans="2:21" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="C5" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="D5" s="14" t="s">
+      <c r="D5" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="E5" s="14" t="s">
         <v>23</v>
       </c>
       <c r="S5" t="s">
         <v>14</v>
       </c>
-      <c r="T5" s="11">
+      <c r="T5" s="10">
         <f>T4/T2</f>
         <v>0.12550057034681941</v>
       </c>
-      <c r="U5" s="9" t="s">
+      <c r="U5" s="8" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B6" s="16" t="s">
+      <c r="B6" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C6" s="17">
+      <c r="C6" s="16">
         <v>13972</v>
       </c>
-      <c r="D6" s="17">
+      <c r="D6" s="16">
         <v>2920</v>
       </c>
-      <c r="E6" s="16"/>
+      <c r="E6" s="15"/>
     </row>
     <row r="7" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C7" s="17">
+      <c r="C7" s="16">
         <v>11750</v>
       </c>
-      <c r="D7" s="17">
+      <c r="D7" s="16">
         <v>1988</v>
       </c>
-      <c r="E7" s="18">
+      <c r="E7" s="17">
         <f t="shared" ref="E7:E22" si="0">(D7-D6)/D6</f>
         <v>-0.31917808219178084</v>
       </c>
     </row>
     <row r="8" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C8" s="17">
+      <c r="C8" s="16">
         <v>14200</v>
       </c>
-      <c r="D8" s="17">
+      <c r="D8" s="16">
         <v>2036</v>
       </c>
-      <c r="E8" s="18">
+      <c r="E8" s="17">
         <f t="shared" si="0"/>
         <v>2.4144869215291749E-2</v>
       </c>
     </row>
     <row r="9" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B9" s="16" t="s">
+      <c r="B9" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="17">
+      <c r="C9" s="16">
         <v>12000</v>
       </c>
-      <c r="D9" s="17">
+      <c r="D9" s="16">
         <v>2150</v>
       </c>
-      <c r="E9" s="18">
+      <c r="E9" s="17">
         <f t="shared" si="0"/>
         <v>5.5992141453831044E-2</v>
       </c>
     </row>
     <row r="10" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B10" s="16" t="s">
+      <c r="B10" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C10" s="17">
+      <c r="C10" s="16">
         <v>11100</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>2063</v>
       </c>
-      <c r="E10" s="18">
+      <c r="E10" s="17">
         <f t="shared" si="0"/>
         <v>-4.046511627906977E-2</v>
       </c>
-      <c r="G10" s="25" t="s">
+      <c r="G10" s="24" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="25"/>
+      <c r="H10" s="24"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B11" s="16" t="s">
+      <c r="B11" s="15" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="17">
+      <c r="C11" s="16">
         <v>17800</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>2445</v>
       </c>
-      <c r="E11" s="18">
+      <c r="E11" s="17">
         <f t="shared" si="0"/>
         <v>0.1851672321861367</v>
       </c>
-      <c r="G11" s="19" t="s">
+      <c r="G11" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="H11" s="20">
+      <c r="H11" s="19">
         <f>AVERAGE(E6:E22)</f>
         <v>4.0115374039580154E-2</v>
       </c>
     </row>
     <row r="12" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="C12" s="17">
+      <c r="C12" s="16">
         <v>20309</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>3125</v>
       </c>
-      <c r="E12" s="18">
+      <c r="E12" s="17">
         <f t="shared" si="0"/>
         <v>0.27811860940695299</v>
       </c>
     </row>
     <row r="13" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="C13" s="17">
+      <c r="C13" s="16">
         <v>8950</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>1556</v>
       </c>
-      <c r="E13" s="18">
+      <c r="E13" s="17">
         <f t="shared" si="0"/>
         <v>-0.50207999999999997</v>
       </c>
-      <c r="G13" s="22" t="s">
+      <c r="G13" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="H13" s="22" t="s">
+      <c r="H13" s="21" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="14" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="C14" s="17">
+      <c r="C14" s="16">
         <v>22705</v>
       </c>
-      <c r="D14" s="17">
+      <c r="D14" s="16">
         <v>2156</v>
       </c>
-      <c r="E14" s="18">
+      <c r="E14" s="17">
         <f t="shared" si="0"/>
         <v>0.38560411311053983</v>
       </c>
-      <c r="G14" s="23">
-        <f>SUM(C6:C21)</f>
-        <v>333832</v>
-      </c>
-      <c r="H14" s="23">
-        <f>SUM(D6:D21)</f>
-        <v>42959</v>
+      <c r="G14" s="22">
+        <f>T2</f>
+        <v>370827</v>
+      </c>
+      <c r="H14" s="22">
+        <f>T4</f>
+        <v>46539</v>
       </c>
     </row>
     <row r="15" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B15" s="16" t="s">
+      <c r="B15" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="17">
+      <c r="C15" s="16">
         <v>20039</v>
       </c>
-      <c r="D15" s="17">
+      <c r="D15" s="16">
         <v>2634</v>
       </c>
-      <c r="E15" s="18">
+      <c r="E15" s="17">
         <f t="shared" si="0"/>
         <v>0.22170686456400743</v>
       </c>
     </row>
     <row r="16" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B16" s="16" t="s">
+      <c r="B16" s="15" t="s">
         <v>34</v>
       </c>
-      <c r="C16" s="17">
+      <c r="C16" s="16">
         <v>25950</v>
       </c>
-      <c r="D16" s="17">
+      <c r="D16" s="16">
         <v>3116</v>
       </c>
-      <c r="E16" s="18">
+      <c r="E16" s="17">
         <f t="shared" si="0"/>
         <v>0.18299164768413059</v>
       </c>
+      <c r="G16" s="21" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="17" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="C17" s="17">
+      <c r="C17" s="16">
         <v>24207</v>
       </c>
-      <c r="D17" s="17">
+      <c r="D17" s="16">
         <v>3253</v>
       </c>
-      <c r="E17" s="18">
+      <c r="E17" s="17">
         <f t="shared" si="0"/>
         <v>4.396662387676508E-2</v>
       </c>
-      <c r="N17" s="3"/>
-      <c r="O17" s="4"/>
-      <c r="S17" s="5"/>
+      <c r="G17" s="26">
+        <f>T5</f>
+        <v>0.12550057034681941</v>
+      </c>
+      <c r="N17" s="2"/>
+      <c r="O17" s="3"/>
+      <c r="S17" s="4"/>
     </row>
     <row r="18" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B18" s="16" t="s">
+      <c r="B18" s="15" t="s">
         <v>24</v>
       </c>
-      <c r="C18" s="17">
+      <c r="C18" s="16">
         <v>29400</v>
       </c>
-      <c r="D18" s="17">
+      <c r="D18" s="16">
         <v>3221</v>
       </c>
-      <c r="E18" s="18">
+      <c r="E18" s="17">
         <f t="shared" si="0"/>
         <v>-9.8370734706424833E-3</v>
       </c>
     </row>
     <row r="19" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B19" s="16" t="s">
+      <c r="B19" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="C19" s="17">
+      <c r="C19" s="16">
         <v>40708</v>
       </c>
-      <c r="D19" s="17">
+      <c r="D19" s="16">
         <v>3479</v>
       </c>
-      <c r="E19" s="18">
+      <c r="E19" s="17">
         <f t="shared" si="0"/>
         <v>8.0099348028562556E-2</v>
       </c>
     </row>
     <row r="20" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B20" s="16" t="s">
+      <c r="B20" s="15" t="s">
         <v>26</v>
       </c>
-      <c r="C20" s="17">
+      <c r="C20" s="16">
         <v>34000</v>
       </c>
-      <c r="D20" s="17">
+      <c r="D20" s="16">
         <v>3707</v>
       </c>
-      <c r="E20" s="18">
+      <c r="E20" s="17">
         <f t="shared" si="0"/>
         <v>6.5536073584363322E-2</v>
       </c>
     </row>
     <row r="21" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="15" t="s">
         <v>27</v>
       </c>
-      <c r="C21" s="17">
+      <c r="C21" s="16">
         <v>26742</v>
       </c>
-      <c r="D21" s="17">
+      <c r="D21" s="16">
         <v>3110</v>
       </c>
-      <c r="E21" s="18">
+      <c r="E21" s="17">
         <f t="shared" si="0"/>
         <v>-0.1610466684650661</v>
       </c>
     </row>
     <row r="22" spans="2:19" x14ac:dyDescent="0.25">
-      <c r="B22" s="16" t="s">
+      <c r="B22" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="17">
+      <c r="C22" s="16">
         <v>36995</v>
       </c>
-      <c r="D22" s="17">
+      <c r="D22" s="16">
         <v>3580</v>
       </c>
-      <c r="E22" s="18">
+      <c r="E22" s="17">
         <f t="shared" si="0"/>
         <v>0.15112540192926044</v>
       </c>
@@ -1186,13 +1195,13 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <f>E4*D4</f>
         <v>25</v>
       </c>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="8"/>
+      <c r="B5" s="7"/>
       <c r="C5" t="s">
         <v>11</v>
       </c>
@@ -1202,13 +1211,13 @@
       <c r="E5">
         <v>30</v>
       </c>
-      <c r="F5" s="6">
+      <c r="F5" s="5">
         <f>E5*D5</f>
         <v>1050</v>
       </c>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="F6" s="7">
+      <c r="F6" s="6">
         <f>SUM(F4:F5)</f>
         <v>1075</v>
       </c>
@@ -1341,7 +1350,7 @@
       <c r="A21" t="s">
         <v>43</v>
       </c>
-      <c r="B21" s="21">
+      <c r="B21" s="20">
         <v>6266</v>
       </c>
       <c r="C21">
@@ -1404,7 +1413,7 @@
       </c>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>47</v>
       </c>
       <c r="E4" t="s">
@@ -1412,7 +1421,7 @@
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A5" s="24" t="s">
+      <c r="A5" s="23" t="s">
         <v>48</v>
       </c>
       <c r="E5" t="s">
@@ -1420,7 +1429,7 @@
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="23" t="s">
         <v>49</v>
       </c>
       <c r="E6" t="s">
@@ -1433,7 +1442,7 @@
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="23" t="s">
         <v>51</v>
       </c>
       <c r="E8" t="s">
@@ -1449,7 +1458,7 @@
       <c r="A10" t="s">
         <v>59</v>
       </c>
-      <c r="I10" s="24" t="s">
+      <c r="I10" s="23" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
change the name of the app
</commit_message>
<xml_diff>
--- a/excl/Calcs for spx.xlsx
+++ b/excl/Calcs for spx.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\toms.druvaskalns\Personal GitHub Projects\JavaApiForShareApp\excl\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F30DFDD1-1A1A-4AA3-9E0A-78F139B4775B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B59F77-EEF3-4C39-9264-493CBABBF9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="601" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15840" tabRatio="601" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="SPX calcs" sheetId="1" r:id="rId1"/>
-    <sheet name="Celeste" sheetId="3" r:id="rId2"/>
-    <sheet name="Money savers" sheetId="2" r:id="rId3"/>
-    <sheet name="Tech" sheetId="4" r:id="rId4"/>
+    <sheet name="protien pie" sheetId="5" r:id="rId2"/>
+    <sheet name="Celeste" sheetId="3" r:id="rId3"/>
+    <sheet name="Money savers" sheetId="2" r:id="rId4"/>
+    <sheet name="Tech" sheetId="4" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="89">
   <si>
     <t>Blitz</t>
   </si>
@@ -257,18 +258,68 @@
   </si>
   <si>
     <t>Enabled account creation for users</t>
+  </si>
+  <si>
+    <t>Ingredient</t>
+  </si>
+  <si>
+    <t>Flour</t>
+  </si>
+  <si>
+    <t>Meat</t>
+  </si>
+  <si>
+    <t>Skyr</t>
+  </si>
+  <si>
+    <t>cheese</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>Protein</t>
+  </si>
+  <si>
+    <t>Kcal</t>
+  </si>
+  <si>
+    <t>Price</t>
+  </si>
+  <si>
+    <t>Chocolate mousse</t>
+  </si>
+  <si>
+    <t>Eggs</t>
+  </si>
+  <si>
+    <t>Sugar</t>
+  </si>
+  <si>
+    <t>Chocolate</t>
+  </si>
+  <si>
+    <t>Fat</t>
+  </si>
+  <si>
+    <t>Portions</t>
+  </si>
+  <si>
+    <t>Per</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="5">
+  <numFmts count="7">
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="#,##0.0000"/>
     <numFmt numFmtId="166" formatCode="_-[$$-409]* #,##0.00_ ;_-[$$-409]* \-#,##0.00\ ;_-[$$-409]* &quot;-&quot;??_ ;_-@_ "/>
     <numFmt numFmtId="167" formatCode="_-* #,##0.00000_-;\-* #,##0.00000_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="168" formatCode="_-[$£-809]* #,##0.00_-;\-[$£-809]* #,##0.00_-;_-[$£-809]* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -390,12 +441,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -432,12 +484,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="167" fontId="0" fillId="4" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="3" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="3" builtinId="4"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Percent" xfId="2" builtinId="5"/>
   </cellStyles>
@@ -743,7 +798,7 @@
   </sheetPr>
   <dimension ref="B1:U24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="I27" sqref="I27"/>
     </sheetView>
   </sheetViews>
@@ -925,10 +980,10 @@
         <f t="shared" si="0"/>
         <v>-4.046511627906977E-2</v>
       </c>
-      <c r="G10" s="26" t="s">
+      <c r="G10" s="28" t="s">
         <v>37</v>
       </c>
-      <c r="H10" s="26"/>
+      <c r="H10" s="28"/>
     </row>
     <row r="11" spans="2:21" x14ac:dyDescent="0.25">
       <c r="B11" s="15" t="s">
@@ -1190,6 +1245,238 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1331DC7-4F15-42F7-97D6-9271C2B8A8EF}">
+  <dimension ref="A1:I14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C17" sqref="C17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>73</v>
+      </c>
+      <c r="B1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C1" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="D1" t="s">
+        <v>79</v>
+      </c>
+      <c r="E1" t="s">
+        <v>86</v>
+      </c>
+      <c r="F1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2">
+        <f>348/2</f>
+        <v>174</v>
+      </c>
+      <c r="C2">
+        <v>50</v>
+      </c>
+      <c r="D2">
+        <v>7.5</v>
+      </c>
+      <c r="F2" s="26">
+        <f>2/(1500/50)</f>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3">
+        <v>155</v>
+      </c>
+      <c r="C3">
+        <v>125</v>
+      </c>
+      <c r="D3">
+        <v>26</v>
+      </c>
+      <c r="F3" s="27">
+        <f>3.5/4</f>
+        <v>0.875</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="C4">
+        <v>50</v>
+      </c>
+      <c r="D4">
+        <v>5</v>
+      </c>
+      <c r="F4" s="27">
+        <f>2/9</f>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>77</v>
+      </c>
+      <c r="B5">
+        <v>52</v>
+      </c>
+      <c r="C5">
+        <v>20</v>
+      </c>
+      <c r="D5">
+        <v>5.9</v>
+      </c>
+      <c r="F5" s="27">
+        <f>2.5/8</f>
+        <v>0.3125</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B6">
+        <f>SUM(B2:B5)</f>
+        <v>411</v>
+      </c>
+      <c r="C6">
+        <f>SUM(C2:C5)</f>
+        <v>245</v>
+      </c>
+      <c r="D6">
+        <f>SUM(D2:D5)</f>
+        <v>44.4</v>
+      </c>
+      <c r="F6" s="26">
+        <f>SUM(F2:F5)</f>
+        <v>1.4763888888888888</v>
+      </c>
+      <c r="I6" s="26"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B10">
+        <f>63*6</f>
+        <v>378</v>
+      </c>
+      <c r="D10">
+        <v>36</v>
+      </c>
+      <c r="E10">
+        <f>4.2*6</f>
+        <v>25.200000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>84</v>
+      </c>
+      <c r="B11">
+        <v>200</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>85</v>
+      </c>
+      <c r="B12">
+        <v>400</v>
+      </c>
+      <c r="D12">
+        <v>5</v>
+      </c>
+      <c r="E12">
+        <f>6.7*4</f>
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <f>SUM(B10:B12)</f>
+        <v>978</v>
+      </c>
+      <c r="C13">
+        <f t="shared" ref="C13:F13" si="0">SUM(C10:C12)</f>
+        <v>0</v>
+      </c>
+      <c r="D13">
+        <f t="shared" si="0"/>
+        <v>41</v>
+      </c>
+      <c r="E13">
+        <f t="shared" si="0"/>
+        <v>52</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>88</v>
+      </c>
+      <c r="B14">
+        <f>B13/B8</f>
+        <v>326</v>
+      </c>
+      <c r="C14">
+        <f t="shared" ref="C14:F14" si="1">C13/3</f>
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <f>D13/B8</f>
+        <v>13.666666666666666</v>
+      </c>
+      <c r="E14">
+        <f>E13/B8</f>
+        <v>17.333333333333332</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3CFFD7C7-06CE-47B6-9A09-47DD80DCF7C2}">
   <dimension ref="B2:I6"/>
   <sheetViews>
@@ -1259,7 +1546,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9ECD8382-CFBB-48E5-BF9F-3DE6EBF9F25C}">
   <dimension ref="A1:C22"/>
   <sheetViews>
@@ -1395,7 +1682,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B65FF673-949D-4E3D-A21C-65A854499F64}">
   <dimension ref="A1:I16"/>
   <sheetViews>

</xml_diff>